<commit_message>
created a report base template and started using of async/await feature in typescript
</commit_message>
<xml_diff>
--- a/AmpedBiz/AmpedBiz.Service.Host/Data/Default/default_suppliers.xlsx
+++ b/AmpedBiz/AmpedBiz.Service.Host/Data/Default/default_suppliers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">smscci_coffee!$A$2:$O$42</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">smscci_coffee!$1:$8</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>SAN MIGUEL INTEGRATED SALES</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>SAN MIGUEL</t>
+  </si>
+  <si>
+    <t>Contact Person</t>
   </si>
 </sst>
 </file>
@@ -943,7 +946,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18050" name="Picture 2"/>
+        <xdr:cNvPr id="18050" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082460000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -989,7 +998,13 @@
     <xdr:ext cx="914400" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="Picture 1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0">
           <a:picLocks noChangeArrowheads="1" noChangeShapeType="1"/>
         </xdr:cNvPicPr>
@@ -1035,7 +1050,13 @@
     <xdr:ext cx="914400" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" hidden="1"/>
+        <xdr:cNvPr id="3" name="Picture 2" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0">
           <a:picLocks noChangeArrowheads="1" noChangeShapeType="1"/>
         </xdr:cNvPicPr>
@@ -1081,7 +1102,13 @@
     <xdr:ext cx="914400" cy="228600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" hidden="1"/>
+        <xdr:cNvPr id="4" name="Picture 3" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0">
           <a:picLocks noChangeArrowheads="1" noChangeShapeType="1"/>
         </xdr:cNvPicPr>
@@ -1417,25 +1444,25 @@
       <selection pane="bottomLeft" activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="10" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="27" customWidth="1"/>
     <col min="3" max="3" width="45" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="4" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,19 +1494,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="45" t="s">
         <v>14</v>
@@ -1488,10 +1515,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:15" s="51" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="51" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="77"/>
       <c r="B7" s="89" t="s">
         <v>2</v>
@@ -1518,7 +1545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="51" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="51" customFormat="1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="77"/>
       <c r="B8" s="89"/>
       <c r="C8" s="90"/>
@@ -1555,7 +1582,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
@@ -1572,7 +1599,7 @@
       <c r="L9" s="75"/>
       <c r="M9" s="76"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="28" t="s">
         <v>7</v>
@@ -1589,7 +1616,7 @@
       <c r="L10" s="39"/>
       <c r="M10" s="59"/>
     </row>
-    <row r="11" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="30" t="s">
         <v>51</v>
@@ -1636,7 +1663,7 @@
         <v>1.0814999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="30" t="s">
         <v>52</v>
@@ -1685,7 +1712,7 @@
         <v>1.0815000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="36" t="s">
         <v>18</v>
@@ -1702,7 +1729,7 @@
       <c r="L13" s="40"/>
       <c r="M13" s="60"/>
     </row>
-    <row r="14" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="29">
         <v>5020170893834</v>
@@ -1748,7 +1775,7 @@
         <v>1.0833333333333333</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
       <c r="B15" s="54"/>
       <c r="C15" s="63"/>
@@ -1763,7 +1790,7 @@
       <c r="L15" s="64"/>
       <c r="M15" s="47"/>
     </row>
-    <row r="16" spans="1:15" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1780,7 +1807,7 @@
       <c r="L16" s="50"/>
       <c r="M16" s="59"/>
     </row>
-    <row r="17" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="29" t="s">
         <v>53</v>
@@ -1830,7 +1857,7 @@
         <v>1.0830026455026456</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="46"/>
       <c r="C18" s="55"/>
@@ -1845,7 +1872,7 @@
       <c r="L18" s="42"/>
       <c r="M18" s="58"/>
     </row>
-    <row r="19" spans="1:15" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>30</v>
       </c>
@@ -1862,7 +1889,7 @@
       <c r="L19" s="50"/>
       <c r="M19" s="59"/>
     </row>
-    <row r="20" spans="1:15" s="73" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" s="73" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="69"/>
       <c r="B20" s="29" t="s">
         <v>54</v>
@@ -1912,7 +1939,7 @@
         <v>1.0845439870863598</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="73" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" s="73" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="69"/>
       <c r="B21" s="29">
         <v>5020170871198</v>
@@ -1960,7 +1987,7 @@
         <v>1.0815677966101696</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="73" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" s="73" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="69"/>
       <c r="B22" s="29">
         <v>5020170883912</v>
@@ -2008,7 +2035,7 @@
         <v>1.0815173527037933</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>10</v>
       </c>
@@ -2025,7 +2052,7 @@
       <c r="L23" s="39"/>
       <c r="M23" s="59"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="28" t="s">
         <v>7</v>
@@ -2042,7 +2069,7 @@
       <c r="L24" s="39"/>
       <c r="M24" s="59"/>
     </row>
-    <row r="25" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="30" t="s">
         <v>55</v>
@@ -2088,7 +2115,7 @@
         <v>1.0863867122834123</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="30" t="s">
         <v>56</v>
@@ -2135,7 +2162,7 @@
         <v>1.082485386447283</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="30" t="s">
         <v>57</v>
@@ -2181,7 +2208,7 @@
         <v>1.0802139037433156</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="28" t="s">
         <v>8</v>
@@ -2198,7 +2225,7 @@
       <c r="L28" s="39"/>
       <c r="M28" s="59"/>
     </row>
-    <row r="29" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="30" t="s">
         <v>58</v>
@@ -2245,7 +2272,7 @@
         <v>1.0842127503419441</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="28" t="s">
         <v>9</v>
@@ -2262,7 +2289,7 @@
       <c r="L30" s="39"/>
       <c r="M30" s="59"/>
     </row>
-    <row r="31" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24"/>
       <c r="B31" s="30" t="s">
         <v>59</v>
@@ -2309,7 +2336,7 @@
         <v>1.0842127503419441</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>20</v>
       </c>
@@ -2326,7 +2353,7 @@
       <c r="L32" s="50"/>
       <c r="M32" s="59"/>
     </row>
-    <row r="33" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
       <c r="B33" s="30" t="s">
         <v>60</v>
@@ -2375,7 +2402,7 @@
         <v>1.0838195295143576</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
       <c r="B34" s="30" t="s">
         <v>61</v>
@@ -2424,7 +2451,7 @@
         <v>1.0863889777837665</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
       <c r="B35" s="30" t="s">
         <v>62</v>
@@ -2474,7 +2501,7 @@
         <v>1.0863889777837665</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="30" t="s">
         <v>63</v>
@@ -2524,7 +2551,7 @@
         <v>1.0863889777837665</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="30" t="s">
         <v>64</v>
@@ -2574,7 +2601,7 @@
         <v>1.0863889777837665</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
       <c r="B38" s="30" t="s">
         <v>65</v>
@@ -2624,7 +2651,7 @@
         <v>1.0863889777837665</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="30">
         <v>5020170897142</v>
@@ -2673,7 +2700,7 @@
         <v>1.0863889777837665</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="68" t="s">
         <v>66</v>
       </c>
@@ -2690,7 +2717,7 @@
       <c r="L40" s="50"/>
       <c r="M40" s="59"/>
     </row>
-    <row r="41" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="30">
         <v>5020170892344</v>
@@ -2734,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="30">
         <v>5020170892346</v>
@@ -2804,46 +2831,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="85" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="85" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="85" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="85" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" style="85" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="85" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="85" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.85546875" style="85" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="85" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="85"/>
+    <col min="1" max="1" width="14.109375" style="85" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="85" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="85" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="85" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="85" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="85" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="85" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="85" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="85" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.88671875" style="85" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" style="85" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="84" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="86"/>
       <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>